<commit_message>
Commit from GitHub Actions (Package Comparison Tool)
</commit_message>
<xml_diff>
--- a/_Cardinality.xlsx
+++ b/_Cardinality.xlsx
@@ -590,7 +590,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>..1</t>
+          <t xml:space="preserve"> ..1</t>
         </is>
       </c>
     </row>
@@ -652,7 +652,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>..*</t>
+          <t xml:space="preserve"> ..*</t>
         </is>
       </c>
     </row>
@@ -809,7 +809,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>..*</t>
+          <t xml:space="preserve"> ..*</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
@@ -823,7 +823,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>..1</t>
+          <t xml:space="preserve"> ..1</t>
         </is>
       </c>
     </row>
@@ -2951,7 +2951,7 @@
       <c r="Z43" t="inlineStr"/>
       <c r="AA43" t="inlineStr">
         <is>
-          <t>..0</t>
+          <t xml:space="preserve"> ..0</t>
         </is>
       </c>
       <c r="AB43" t="inlineStr"/>
@@ -3487,7 +3487,7 @@
       <c r="N51" t="inlineStr"/>
       <c r="O51" t="inlineStr">
         <is>
-          <t>..0</t>
+          <t xml:space="preserve"> ..0</t>
         </is>
       </c>
       <c r="P51" t="inlineStr"/>
@@ -3632,7 +3632,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>..1</t>
+          <t xml:space="preserve"> ..1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -3645,7 +3645,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>..1</t>
+          <t xml:space="preserve"> ..1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -3658,7 +3658,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>..4</t>
+          <t xml:space="preserve"> ..4</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -3671,7 +3671,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>..1</t>
+          <t xml:space="preserve"> ..1</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -3684,7 +3684,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>..1</t>
+          <t xml:space="preserve"> ..1</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
@@ -3697,7 +3697,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>..1</t>
+          <t xml:space="preserve"> ..1</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -3710,7 +3710,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>..1</t>
+          <t xml:space="preserve"> ..1</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
@@ -3724,7 +3724,7 @@
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr">
         <is>
-          <t>..1</t>
+          <t xml:space="preserve"> ..1</t>
         </is>
       </c>
     </row>
@@ -3763,7 +3763,7 @@
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr">
         <is>
-          <t>..1</t>
+          <t xml:space="preserve"> ..1</t>
         </is>
       </c>
     </row>
@@ -3898,7 +3898,7 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>..1</t>
+          <t xml:space="preserve"> ..1</t>
         </is>
       </c>
     </row>
@@ -4001,7 +4001,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>..1</t>
+          <t xml:space="preserve"> ..1</t>
         </is>
       </c>
     </row>
@@ -4013,7 +4013,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>..1</t>
+          <t xml:space="preserve"> ..1</t>
         </is>
       </c>
     </row>
@@ -4025,7 +4025,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>..4</t>
+          <t xml:space="preserve"> ..4</t>
         </is>
       </c>
     </row>
@@ -4037,7 +4037,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>..1</t>
+          <t xml:space="preserve"> ..1</t>
         </is>
       </c>
     </row>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>..1</t>
+          <t xml:space="preserve"> ..1</t>
         </is>
       </c>
     </row>
@@ -4235,7 +4235,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>..*</t>
+          <t xml:space="preserve"> ..*</t>
         </is>
       </c>
     </row>
@@ -4757,7 +4757,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>..1</t>
+          <t xml:space="preserve"> ..1</t>
         </is>
       </c>
     </row>
@@ -4819,7 +4819,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>..1</t>
+          <t xml:space="preserve"> ..1</t>
         </is>
       </c>
     </row>

</xml_diff>